<commit_message>
CA Visibility report,  Base page , Excel test data handler, deleted write to excel method
</commit_message>
<xml_diff>
--- a/CompetitiveAnalysis.xlsx
+++ b/CompetitiveAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wasim\git\DACAutomation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rahuln\git\DACAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5005815C-B10E-43E7-A456-3523EA8CC134}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C26DA3-FC6C-4081-8BDD-E0CA70989068}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="7290" xr2:uid="{66D78547-9A11-428C-B5AF-16FD7C7547B7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="5895" xr2:uid="{66D78547-9A11-428C-B5AF-16FD7C7547B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculation Verification" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -42,43 +42,118 @@
     <t>ScreenCapture needed</t>
   </si>
   <si>
-    <t>id:5000</t>
-  </si>
-  <si>
     <t>CA Calculation Verification</t>
   </si>
   <si>
-    <t>Navigate to visibility page</t>
-  </si>
-  <si>
     <t>Scroll down to over view report</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>Over view report loads</t>
-  </si>
-  <si>
     <t>Capture visibility scores</t>
   </si>
   <si>
-    <t>Visibility scores stored for calculations</t>
-  </si>
-  <si>
     <t>Export Over view report</t>
   </si>
   <si>
-    <t>Capture Accuracy scores</t>
-  </si>
-  <si>
-    <t>Accuracy scores stored for calculations</t>
-  </si>
-  <si>
     <t>Navigate to Accuracy page</t>
   </si>
   <si>
-    <t>Calculations successfully stored in result file</t>
+    <t>verifyOverviewReportnExport</t>
+  </si>
+  <si>
+    <t>id:2</t>
+  </si>
+  <si>
+    <t>verifyOverviewReportnTooltip</t>
+  </si>
+  <si>
+    <t>id:3</t>
+  </si>
+  <si>
+    <t>id:4</t>
+  </si>
+  <si>
+    <t>verifySiteTablenExport</t>
+  </si>
+  <si>
+    <t>verifyFilteringReports</t>
+  </si>
+  <si>
+    <t>id:1</t>
+  </si>
+  <si>
+    <t>id:5</t>
+  </si>
+  <si>
+    <t>Log into TransparenSee</t>
+  </si>
+  <si>
+    <t>Navigate to CA Visibility page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify Global filter is loaded </t>
+  </si>
+  <si>
+    <t>Navigation page is loaded correctly</t>
+  </si>
+  <si>
+    <t>Global filter should load</t>
+  </si>
+  <si>
+    <t>Apply filter for-&gt; US,Illinois,Chicago,53 W Jackson Blvd Ste 1264</t>
+  </si>
+  <si>
+    <t>Click Apply Filter</t>
+  </si>
+  <si>
+    <t>Overview report should load after filter is applied</t>
+  </si>
+  <si>
+    <t>Overview report should be exported properly</t>
+  </si>
+  <si>
+    <t>Both scores should match</t>
+  </si>
+  <si>
+    <t>Scroll down to visibility score history graph</t>
+  </si>
+  <si>
+    <t>Read exported excel and fetch scores for each competitor</t>
+  </si>
+  <si>
+    <t>Compare excel Overall score in export with Overview report Score for each competitor</t>
+  </si>
+  <si>
+    <t>Mouse over to latest data point</t>
+  </si>
+  <si>
+    <t>Read values score from tooltip for each competitor</t>
+  </si>
+  <si>
+    <t>Read scores for each competitor from Overview report</t>
+  </si>
+  <si>
+    <t>Compare scores for each competitor</t>
+  </si>
+  <si>
+    <t>Visibility graph should be loaded</t>
+  </si>
+  <si>
+    <t>Overview report should be visible</t>
+  </si>
+  <si>
+    <t>Check overview report is visible</t>
+  </si>
+  <si>
+    <t>Check visibility graph is visible</t>
+  </si>
+  <si>
+    <t>Check site table is visible</t>
+  </si>
+  <si>
+    <t>Scroll down to site table</t>
   </si>
 </sst>
 </file>
@@ -433,16 +508,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD74DF37-6EE2-4904-B097-EF831BBF89C5}">
-  <dimension ref="A1:E673"/>
+  <dimension ref="A1:E672"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1"/>
     <col min="3" max="3" width="76.5703125" customWidth="1"/>
     <col min="4" max="4" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.7109375" customWidth="1"/>
@@ -467,89 +542,196 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="A6" t="s">
         <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>16</v>
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D19" s="1"/>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C37" s="1"/>
-    </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C45" s="1"/>
-    </row>
-    <row r="432" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C432" s="1"/>
-    </row>
-    <row r="639" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C639" s="1"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="1"/>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="1"/>
+    </row>
+    <row r="431" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C431" s="1"/>
+    </row>
+    <row r="638" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C638" s="1"/>
+    </row>
+    <row r="640" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C640" s="1"/>
     </row>
     <row r="641" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C641" s="1"/>
@@ -557,23 +739,23 @@
     <row r="642" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C642" s="1"/>
     </row>
-    <row r="643" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C643" s="1"/>
-    </row>
-    <row r="645" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C645" s="1"/>
-    </row>
-    <row r="647" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C647" s="1"/>
-    </row>
-    <row r="649" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C649" s="1"/>
-    </row>
-    <row r="654" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C654" s="1"/>
-    </row>
-    <row r="658" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C658" s="1"/>
+    <row r="644" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C644" s="1"/>
+    </row>
+    <row r="646" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C646" s="1"/>
+    </row>
+    <row r="648" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C648" s="1"/>
+    </row>
+    <row r="653" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C653" s="1"/>
+    </row>
+    <row r="657" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C657" s="1"/>
+    </row>
+    <row r="659" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C659" s="1"/>
     </row>
     <row r="660" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C660" s="1"/>
@@ -581,20 +763,17 @@
     <row r="661" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C661" s="1"/>
     </row>
-    <row r="662" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C662" s="1"/>
-    </row>
-    <row r="664" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C664" s="1"/>
-    </row>
-    <row r="666" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C666" s="1"/>
-    </row>
-    <row r="668" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C668" s="1"/>
-    </row>
-    <row r="673" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C673" s="1"/>
+    <row r="663" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C663" s="1"/>
+    </row>
+    <row r="665" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C665" s="1"/>
+    </row>
+    <row r="667" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C667" s="1"/>
+    </row>
+    <row r="672" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C672" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
multiple changes on fixing evidence creation. Need further work on all images not appearing
</commit_message>
<xml_diff>
--- a/CompetitiveAnalysis.xlsx
+++ b/CompetitiveAnalysis.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4CCF2272-80B2-4F5A-B359-9A89E8812BA0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A4660F18-9AD6-4225-94C6-8B4CB02E7ABB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="5895" activeTab="1" xr2:uid="{66D78547-9A11-428C-B5AF-16FD7C7547B7}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>Scroll down to site table</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -781,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9940159-E932-4248-B5B6-D6CE46539389}">
   <dimension ref="A1:E672"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,10 +915,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -923,7 +926,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>40</v>
       </c>
@@ -931,32 +934,35 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -964,27 +970,30 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Fixed issues with Test evidence
Changed test evidence , read excel class
Modified CA test classes with sample screen capture
</commit_message>
<xml_diff>
--- a/CompetitiveAnalysis.xlsx
+++ b/CompetitiveAnalysis.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A4660F18-9AD6-4225-94C6-8B4CB02E7ABB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A5C9030A-3FD0-4DE8-A8C2-415A9AC5858E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="5895" activeTab="1" xr2:uid="{66D78547-9A11-428C-B5AF-16FD7C7547B7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Calculation Verification" sheetId="1" r:id="rId1"/>
+    <sheet name="Visibility testcases" sheetId="1" r:id="rId1"/>
     <sheet name="Review testcases" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M17"/>
+  <oleSize ref="C16:D32"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -154,6 +154,24 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Navigate to CA Review page</t>
+  </si>
+  <si>
+    <t>Check Review graph is visible</t>
+  </si>
+  <si>
+    <t>Review graph should be loaded</t>
+  </si>
+  <si>
+    <t>Scroll down to Review score history graph</t>
+  </si>
+  <si>
+    <t>Review Site table should be loaded</t>
+  </si>
+  <si>
+    <t>Capture Review scores</t>
   </si>
 </sst>
 </file>
@@ -510,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD74DF37-6EE2-4904-B097-EF831BBF89C5}">
   <dimension ref="A1:E672"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C37" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="B24" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,13 +629,13 @@
       <c r="D12" t="s">
         <v>38</v>
       </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>6</v>
-      </c>
-      <c r="E13" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -784,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9940159-E932-4248-B5B6-D6CE46539389}">
   <dimension ref="A1:E672"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +847,7 @@
     </row>
     <row r="4" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
@@ -885,14 +903,14 @@
       <c r="D12" t="s">
         <v>38</v>
       </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>6</v>
       </c>
-      <c r="E13" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="14" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
@@ -928,15 +946,18 @@
     </row>
     <row r="19" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>46</v>
+      </c>
+      <c r="E19" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
@@ -948,9 +969,6 @@
       <c r="C22" t="s">
         <v>34</v>
       </c>
-      <c r="E22" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="23" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
@@ -984,13 +1002,16 @@
       <c r="C29" t="s">
         <v>9</v>
       </c>
+      <c r="D29" t="s">
+        <v>48</v>
+      </c>
       <c r="E29" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>